<commit_message>
Add png file for Tir
</commit_message>
<xml_diff>
--- a/04 - Tir.xlsx
+++ b/04 - Tir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\MaktabSharif\Works\Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C8769A-D5E2-4F4D-885C-25BAC1410A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1E15EF-A5E8-4D55-9730-AE3A70558D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{FF2BF689-5E91-4292-9B13-39FB55D30CFD}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>جمعه</t>
   </si>
   <si>
-    <t>خرداد</t>
-  </si>
-  <si>
     <t>بازگیر</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">تقویم ضبط </t>
+  </si>
+  <si>
+    <t>تیر</t>
   </si>
 </sst>
 </file>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CBB7FF-EFC4-4E2B-95A1-B7CF7FA5FC2B}">
   <dimension ref="E3:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,7 +532,7 @@
   <sheetData>
     <row r="3" spans="5:20" ht="28.5" x14ac:dyDescent="0.65">
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="5:20" ht="25" thickBot="1" x14ac:dyDescent="0.4">
@@ -558,22 +558,22 @@
         <v>0</v>
       </c>
       <c r="M5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="5:20" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -590,10 +590,10 @@
     </row>
     <row r="7" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E7" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M7" s="8"/>
     </row>
@@ -623,13 +623,13 @@
     </row>
     <row r="9" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E9" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M9" s="8"/>
     </row>
@@ -659,13 +659,13 @@
     </row>
     <row r="11" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E11" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M11" s="8"/>
     </row>
@@ -695,13 +695,13 @@
     </row>
     <row r="13" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E13" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M13" s="8"/>
     </row>
@@ -731,7 +731,7 @@
     </row>
     <row r="15" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H15" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="5:20" ht="24.5" x14ac:dyDescent="0.35">

</xml_diff>